<commit_message>
Fix ModuleNotFoundError by adding project path
</commit_message>
<xml_diff>
--- a/logs/dependencies.xlsx
+++ b/logs/dependencies.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CB8666-A84C-3245-B168-9E66C0302DFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4BDE1C-887B-0E4A-85C5-1EFBEF52BDDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="2940" windowWidth="28040" windowHeight="17440" xr2:uid="{9374D456-37F1-F741-A2F7-0666F828AF29}"/>
+    <workbookView xWindow="6580" yWindow="1460" windowWidth="25900" windowHeight="11940" xr2:uid="{9374D456-37F1-F741-A2F7-0666F828AF29}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="start" sheetId="3" r:id="rId1"/>
+    <sheet name="error" sheetId="5" r:id="rId2"/>
+    <sheet name="py" sheetId="4" r:id="rId3"/>
+    <sheet name="proto" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>client.py</t>
   </si>
@@ -93,39 +96,146 @@
     <t>toolchain.py</t>
   </si>
   <si>
-    <t>$ python3 replace_args.py
-$ sudo pip3 install sqlalchemy
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Dependecies</t>
+  </si>
+  <si>
+    <t>main.py</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>datastore.proto</t>
+  </si>
+  <si>
+    <t>deepsmith.proto</t>
+  </si>
+  <si>
+    <t>generator.proto</t>
+  </si>
+  <si>
+    <t>harness.proto</t>
+  </si>
+  <si>
+    <t>service.proto</t>
+  </si>
+  <si>
+    <t>clgen.proto</t>
+  </si>
+  <si>
+    <t>corpus.proto</t>
+  </si>
+  <si>
+    <t>internal.proto</t>
+  </si>
+  <si>
+    <t>model.proto</t>
+  </si>
+  <si>
+    <t>sampler.proto</t>
+  </si>
+  <si>
+    <t>telemetry.proto</t>
+  </si>
+  <si>
+    <t>$ protoc --proto_path=/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/clgen/proto/ --python_out=/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/clgen/proto/ x.proto</t>
+  </si>
+  <si>
+    <t>$ protoc --proto_path=/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/deepsmith/proto/ --python_out=/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/deepsmith/proto/ x.proto</t>
+  </si>
+  <si>
+    <t># Setting PATH for Python Project
+export PATH=$PATH:~/Desktop/Rabin/deep-smith/phd/ #DeepSmith</t>
+  </si>
+  <si>
+    <t>clgen</t>
+  </si>
+  <si>
+    <t>~/.bash_profile
+source ~/.bash_profile</t>
+  </si>
+  <si>
+    <t>$ sudo pip3 install sqlalchemy
 $ sudo pip3 install pytest
 $ sudo pip3 install absl-py
-$ sudo pip3 install grpcio grpcio-tools</t>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Dependecies</t>
-  </si>
-  <si>
-    <t>main.py</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Status</t>
+$ sudo pip3 install grpcio grpcio-tools
+…</t>
+  </si>
+  <si>
+    <t>ModuleNotFoundError: No module named 'deeplearning'</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Solved Error</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Solved By</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    from deeplearning.deepsmith.proto import datastore_pb2
+ImportError: cannot import name 'datastore_pb2' from 'deeplearning.deepsmith.proto' (unknown location)</t>
+  </si>
+  <si>
+    <t>Add project path in bash_profile</t>
+  </si>
+  <si>
+    <t>Install dependencies with sudo pip3</t>
+  </si>
+  <si>
+    <t>Import error</t>
+  </si>
+  <si>
+    <t>Project Path</t>
+  </si>
+  <si>
+    <t>Python Version</t>
+  </si>
+  <si>
+    <t>SyntaxError: invalid syntax</t>
+  </si>
+  <si>
+    <t>Use python v3</t>
+  </si>
+  <si>
+    <t># Setting PATH for Python 3
+export PATH=$PATH:~/Library/Frameworks/Python.framework/Versions/3.7/bin/</t>
+  </si>
+  <si>
+    <t>$ python3 --version
+Python 3.7.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +253,20 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -181,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,19 +315,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,11 +675,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E2F061-ACDE-A946-B94B-1A9F4FF055ED}">
-  <dimension ref="A2:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B7613-A075-744E-A837-EFBEF09CB85C}">
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="13"/>
+    <col min="3" max="3" width="54.1640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="70.83203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B47C618-EC93-794D-BF43-0862D74A4AB5}">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="80.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="7"/>
+    <col min="4" max="4" width="30.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D4A832-FE4B-1847-8459-FFA33D6F687C}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,223 +870,356 @@
     <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E2F061-ACDE-A946-B94B-1A9F4FF055ED}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="138.5" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="D2" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:A26"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A10:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix some dependices and improt issue.
</commit_message>
<xml_diff>
--- a/logs/dependencies.xlsx
+++ b/logs/dependencies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdrafiqulrabin/Desktop/Rabin/forkdeepsmith/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BB4E09-FBA5-444C-B28B-6D4A5663643F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D28E6A-72AC-0E44-B271-DA70E12901B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="1760" windowWidth="25900" windowHeight="11940" xr2:uid="{9374D456-37F1-F741-A2F7-0666F828AF29}"/>
+    <workbookView xWindow="5940" yWindow="3420" windowWidth="25900" windowHeight="11940" xr2:uid="{9374D456-37F1-F741-A2F7-0666F828AF29}"/>
   </bookViews>
   <sheets>
     <sheet name="start" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="py" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
   <si>
     <t>client.py</t>
   </si>
@@ -147,17 +148,6 @@
   </si>
   <si>
     <t>clgen</t>
-  </si>
-  <si>
-    <t>~/.bash_profile
-source ~/.bash_profile</t>
-  </si>
-  <si>
-    <t>$ sudo pip3 install sqlalchemy
-$ sudo pip3 install pytest
-$ sudo pip3 install absl-py
-$ sudo pip3 install grpcio grpcio-tools
-…</t>
   </si>
   <si>
     <t>ModuleNotFoundError: No module named 'deeplearning'</t>
@@ -201,10 +191,6 @@
   <si>
     <t># Setting PATH for Python 3
 export PATH=$PATH:~/Library/Frameworks/Python.framework/Versions/3.7/bin/</t>
-  </si>
-  <si>
-    <t>$ python3 --version
-Python 3.7.0</t>
   </si>
   <si>
     <t>Installing protoc</t>
@@ -251,6 +237,58 @@
     <t># Setting PATH for Python Project
 export PYTHONPATH=~/Desktop/Rabin/deep_smith/phd
 export PATH=$PATH:$PYTHONPATH/</t>
+  </si>
+  <si>
+    <t>$ python3 --version
+Python 3.7.2</t>
+  </si>
+  <si>
+    <t>labm8</t>
+  </si>
+  <si>
+    <t>lockfile.proto</t>
+  </si>
+  <si>
+    <t>logging.proto</t>
+  </si>
+  <si>
+    <t>test_protos.proto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ protoc --proto_path=/Users/mdrafiqulrabin/Desktop/Rabin/deep_smith/phd/  --python_out=/Users/mdrafiqulrabin/Desktop/Rabin/deep_smith/phd/ /Users/mdrafiqulrabin/Desktop/Rabin/deep_smith/phd/labm8/proto/x.proto </t>
+  </si>
+  <si>
+    <t>Addditional Info</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>FileNotFoundError: [Errno 2] No such file or directory: 'deeplearning/deepsmith/tests/data/datastores'</t>
+  </si>
+  <si>
+    <t>$ sudo pip3 install x
+…</t>
+  </si>
+  <si>
+    <t>$ vi ~/.bash_profile
+...
+$ source ~/.bash_profile</t>
+  </si>
+  <si>
+    <t>Don't install 'labm8' by pip3, its already in /php/labm8 folder.</t>
+  </si>
+  <si>
+    <t>[Don't install 'labm8' by pip3, its already in /php/labm8 folder.]</t>
+  </si>
+  <si>
+    <t>pathlib.Path('deeplearning/deepsmith/tests/data/datastores') to pathlib.Path('tests/data/datastores') in conftest.py</t>
+  </si>
+  <si>
+    <t>ERROR at setup of ... [sqlite_memory]</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -281,18 +319,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -327,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -336,12 +374,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,63 +383,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,114 +769,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B7613-A075-744E-A837-EFBEF09CB85C}">
-  <dimension ref="A2:F10"/>
+  <dimension ref="A2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="12"/>
-    <col min="2" max="2" width="10.83203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="54.1640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="69.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="7.1640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="69.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="14"/>
+    <col min="12" max="12" width="15.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.83203125" style="14"/>
+    <col min="17" max="17" width="13.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="14"/>
+    <col min="19" max="19" width="14.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" s="17" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="25"/>
-      <c r="C4" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="18" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="E4" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="25"/>
-      <c r="C5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" s="17" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="17" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="E7" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:11" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A10:B10"/>
@@ -846,91 +908,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B47C618-EC93-794D-BF43-0862D74A4AB5}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="83.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="7"/>
-    <col min="4" max="4" width="30.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="87.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="53.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="A7" s="14">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="B7" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>7</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,15 +1047,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E2F061-ACDE-A946-B94B-1A9F4FF055ED}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="138.5" customWidth="1"/>
     <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
@@ -957,174 +1065,218 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="21" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="20"/>
+    <row r="4" spans="1:4" s="12" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
-        <v>64</v>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="28"/>
+      <c r="B18" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="28"/>
+      <c r="B19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="28"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="28"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="B23" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="B24" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="28"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="A13:A20"/>
     <mergeCell ref="D13:D20"/>
     <mergeCell ref="D6:D12"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="D21:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1132,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D4A832-FE4B-1847-8459-FFA33D6F687C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,154 +1295,180 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="119" customWidth="1"/>
     <col min="4" max="4" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="E3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="26"/>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="26"/>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="C10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="26"/>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
+      <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="26"/>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
+      <c r="A17" s="26"/>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="26"/>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
+      <c r="A19" s="26"/>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
+      <c r="A20" s="26"/>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
+      <c r="A21" s="26"/>
       <c r="B21" t="s">
         <v>18</v>
       </c>

</xml_diff>